<commit_message>
DB - Favorite&Recent(command 파일 추가)
</commit_message>
<xml_diff>
--- a/src/test/DB/table.xlsx
+++ b/src/test/DB/table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\git\Leggo_final\src\test\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahnus\git\Leggo_final\src\test\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC0582-B026-4090-96DA-F96AF0500C2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18330" windowHeight="9750"/>
+    <workbookView xWindow="-8148" yWindow="2616" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="주차장" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="299">
   <si>
     <t>주차장</t>
   </si>
@@ -439,9 +440,6 @@
     <t>장소 코드</t>
   </si>
   <si>
-    <t>visit_code</t>
-  </si>
-  <si>
     <t>favorite_code</t>
   </si>
   <si>
@@ -495,12 +493,6 @@
       </rPr>
       <t>HECK</t>
     </r>
-  </si>
-  <si>
-    <t>방문 횟수</t>
-  </si>
-  <si>
-    <t>visit_num</t>
   </si>
   <si>
     <t>위도</t>
@@ -1800,12 +1792,60 @@
     <t>varchar2</t>
     <phoneticPr fontId="33" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>장소</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 이름</t>
+    </r>
+    <phoneticPr fontId="33" type="noConversion"/>
+  </si>
+  <si>
+    <t>location_name</t>
+    <phoneticPr fontId="33" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar2</t>
+    <phoneticPr fontId="33" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>주차장</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 코드</t>
+    </r>
+    <phoneticPr fontId="33" type="noConversion"/>
+  </si>
+  <si>
+    <t>parking_code</t>
+    <phoneticPr fontId="33" type="noConversion"/>
+  </si>
+  <si>
+    <t>recent_code</t>
+    <phoneticPr fontId="33" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="46">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="48">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2078,6 +2118,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2308,7 +2360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2542,23 +2594,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2582,6 +2618,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2593,6 +2645,11 @@
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2808,51 +2865,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B1:Y983"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="25.140625" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" customWidth="1"/>
+    <col min="8" max="8" width="29.88671875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="25.109375" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" customWidth="1"/>
+    <col min="21" max="21" width="16.88671875" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="136"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="130"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="128" t="s">
+      <c r="H2" s="125" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="133"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
     </row>
     <row r="3" spans="2:24" ht="15.75" customHeight="1">
       <c r="B3" s="96" t="s">
@@ -2889,7 +2946,7 @@
     </row>
     <row r="4" spans="2:24" ht="15.75" customHeight="1">
       <c r="B4" s="111" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C4" s="109" t="s">
         <v>9</v>
@@ -2908,7 +2965,7 @@
         <v>110</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>10</v>
@@ -2939,7 +2996,7 @@
       </c>
       <c r="F5" s="100"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="77" t="s">
         <v>109</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -2948,11 +3005,11 @@
       <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="19">
         <v>20</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M5" s="1"/>
       <c r="T5" s="1"/>
@@ -2976,20 +3033,20 @@
       </c>
       <c r="F6" s="100"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>24</v>
+      <c r="H6" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="I6" s="81" t="s">
+        <v>297</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="7">
+        <v>7</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="M6" s="6"/>
       <c r="T6" s="6"/>
@@ -3000,7 +3057,7 @@
     </row>
     <row r="7" spans="2:24" ht="15.75" customHeight="1">
       <c r="B7" s="114" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C7" s="94" t="s">
         <v>44</v>
@@ -3013,21 +3070,19 @@
       </c>
       <c r="F7" s="115"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="39" t="s">
-        <v>24</v>
-      </c>
+      <c r="H7" s="80" t="s">
+        <v>293</v>
+      </c>
+      <c r="I7" s="147" t="s">
+        <v>294</v>
+      </c>
+      <c r="J7" s="147" t="s">
+        <v>295</v>
+      </c>
+      <c r="K7" s="149">
+        <v>60</v>
+      </c>
+      <c r="L7" s="8"/>
       <c r="M7" s="6"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
@@ -3035,9 +3090,9 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
     </row>
-    <row r="8" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="8" spans="2:24" ht="15.75" customHeight="1">
       <c r="B8" s="114" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C8" s="94" t="s">
         <v>47</v>
@@ -3050,15 +3105,19 @@
       </c>
       <c r="F8" s="115"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="I8" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43" t="s">
+      <c r="H8" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="39" t="s">
         <v>24</v>
       </c>
       <c r="M8" s="6"/>
@@ -3068,7 +3127,7 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
     </row>
-    <row r="9" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="9" spans="2:24" ht="15.75" customHeight="1">
       <c r="B9" s="113" t="s">
         <v>50</v>
       </c>
@@ -3083,11 +3142,21 @@
       </c>
       <c r="F9" s="100"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="H9" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>24</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -3116,13 +3185,21 @@
       </c>
       <c r="F10" s="100"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="128" t="s">
-        <v>105</v>
-      </c>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="130"/>
+      <c r="H10" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="148" t="s">
+        <v>295</v>
+      </c>
+      <c r="K10" s="42">
+        <v>100</v>
+      </c>
+      <c r="L10" s="43" t="s">
+        <v>24</v>
+      </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -3136,9 +3213,9 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="2:24" ht="15.75" customHeight="1">
+    <row r="11" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
       <c r="B11" s="116" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C11" s="94" t="s">
         <v>58</v>
@@ -3151,21 +3228,11 @@
       </c>
       <c r="F11" s="100"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -3179,7 +3246,7 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="2:24" ht="15.75" customHeight="1">
+    <row r="12" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
       <c r="B12" s="113" t="s">
         <v>35</v>
       </c>
@@ -3194,19 +3261,13 @@
       </c>
       <c r="F12" s="100"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="19">
-        <v>30</v>
-      </c>
-      <c r="L12" s="8"/>
+      <c r="H12" s="125" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="140"/>
+      <c r="J12" s="140"/>
+      <c r="K12" s="140"/>
+      <c r="L12" s="141"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -3235,20 +3296,20 @@
       </c>
       <c r="F13" s="120"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="77" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="19">
-        <v>20</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>81</v>
+      <c r="H13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -3271,16 +3332,16 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="77" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>125</v>
+        <v>110</v>
+      </c>
+      <c r="I14" s="81" t="s">
+        <v>298</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K14" s="19">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="6"/>
@@ -3297,28 +3358,28 @@
       <c r="X14" s="6"/>
     </row>
     <row r="15" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="129"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="130"/>
+      <c r="C15" s="140"/>
+      <c r="D15" s="140"/>
+      <c r="E15" s="140"/>
+      <c r="F15" s="141"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="J15" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>24</v>
+      <c r="H15" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="19">
+        <v>20</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -3333,7 +3394,7 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="16" spans="2:24" ht="15.75" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
@@ -3350,20 +3411,20 @@
         <v>7</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="J16" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" s="43" t="s">
-        <v>24</v>
+      <c r="H16" s="80" t="s">
+        <v>296</v>
+      </c>
+      <c r="I16" s="81" t="s">
+        <v>297</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="19">
+        <v>7</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -3378,7 +3439,7 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="17" spans="2:24" ht="15.75" customHeight="1">
       <c r="B17" s="105" t="s">
         <v>8</v>
       </c>
@@ -3395,11 +3456,19 @@
         <v>81</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
+      <c r="H17" s="80" t="s">
+        <v>293</v>
+      </c>
+      <c r="I17" s="147" t="s">
+        <v>294</v>
+      </c>
+      <c r="J17" s="147" t="s">
+        <v>295</v>
+      </c>
+      <c r="K17" s="149">
+        <v>60</v>
+      </c>
+      <c r="L17" s="8"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -3428,13 +3497,21 @@
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="140" t="s">
-        <v>104</v>
-      </c>
-      <c r="I18" s="141"/>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141"/>
-      <c r="L18" s="142"/>
+      <c r="H18" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="39" t="s">
+        <v>24</v>
+      </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -3448,7 +3525,7 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="2:24" ht="15.75" customHeight="1">
+    <row r="19" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
       <c r="B19" s="5" t="s">
         <v>86</v>
       </c>
@@ -3463,20 +3540,20 @@
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="K19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="27" t="s">
-        <v>7</v>
+      <c r="H19" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="43" t="s">
+        <v>24</v>
       </c>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
@@ -3491,7 +3568,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="2:24" ht="15.75" customHeight="1">
+    <row r="20" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
       <c r="B20" s="5" t="s">
         <v>90</v>
       </c>
@@ -3506,21 +3583,11 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="16">
-        <v>20</v>
-      </c>
-      <c r="L20" s="29" t="s">
-        <v>81</v>
-      </c>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -3549,19 +3616,13 @@
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="16">
-        <v>20</v>
-      </c>
-      <c r="L21" s="29"/>
+      <c r="H21" s="134" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="135"/>
+      <c r="J21" s="135"/>
+      <c r="K21" s="135"/>
+      <c r="L21" s="136"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -3575,7 +3636,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
+    <row r="22" spans="2:24" ht="15.75" customHeight="1">
       <c r="B22" s="5" t="s">
         <v>97</v>
       </c>
@@ -3590,20 +3651,20 @@
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="I22" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="J22" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="34">
-        <v>50</v>
-      </c>
-      <c r="L22" s="35" t="s">
-        <v>123</v>
+      <c r="H22" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>7</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -3633,13 +3694,21 @@
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="H23" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="16">
+        <v>20</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>81</v>
+      </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -3668,6 +3737,19 @@
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="1"/>
+      <c r="H24" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="16">
+        <v>20</v>
+      </c>
+      <c r="L24" s="29"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -3683,6 +3765,21 @@
     </row>
     <row r="25" spans="2:24" ht="15.75" customHeight="1" thickBot="1">
       <c r="G25" s="1"/>
+      <c r="H25" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="34">
+        <v>50</v>
+      </c>
+      <c r="L25" s="35" t="s">
+        <v>122</v>
+      </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -3697,14 +3794,21 @@
       <c r="X25" s="6"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" customHeight="1">
-      <c r="B26" s="137" t="s">
+      <c r="B26" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="139"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="133"/>
       <c r="G26" s="6"/>
+      <c r="H26" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -3757,7 +3861,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="124" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G28" s="6"/>
       <c r="M28" s="6"/>
@@ -4162,13 +4266,13 @@
       <c r="T47" s="6"/>
     </row>
     <row r="48" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B48" s="128" t="s">
+      <c r="B48" s="125" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="132"/>
-      <c r="D48" s="132"/>
-      <c r="E48" s="132"/>
-      <c r="F48" s="133"/>
+      <c r="C48" s="126"/>
+      <c r="D48" s="126"/>
+      <c r="E48" s="126"/>
+      <c r="F48" s="127"/>
       <c r="M48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
@@ -4356,7 +4460,7 @@
         <v>93</v>
       </c>
       <c r="D55" s="79" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E55" s="12">
         <v>50</v>
@@ -4490,11 +4594,11 @@
     </row>
     <row r="65" spans="2:25" ht="15.75" customHeight="1">
       <c r="G65" s="6"/>
-      <c r="T65" s="125"/>
-      <c r="U65" s="126"/>
-      <c r="V65" s="126"/>
-      <c r="W65" s="126"/>
-      <c r="X65" s="126"/>
+      <c r="T65" s="137"/>
+      <c r="U65" s="138"/>
+      <c r="V65" s="138"/>
+      <c r="W65" s="138"/>
+      <c r="X65" s="138"/>
     </row>
     <row r="66" spans="2:25" ht="15.75" customHeight="1">
       <c r="G66" s="6"/>
@@ -4639,11 +4743,6 @@
       <c r="E76" s="61"/>
       <c r="F76" s="60"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="56"/>
-      <c r="I76" s="21"/>
-      <c r="J76" s="21"/>
-      <c r="K76" s="22"/>
-      <c r="L76" s="6"/>
       <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
@@ -4664,11 +4763,6 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
-      <c r="H77" s="54"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="6"/>
       <c r="M77" s="6"/>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
@@ -4689,11 +4783,6 @@
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
       <c r="M78" s="6"/>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
@@ -4714,10 +4803,10 @@
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
+      <c r="H79" s="56"/>
+      <c r="I79" s="21"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="22"/>
       <c r="L79" s="6"/>
       <c r="M79" s="6"/>
       <c r="N79" s="6"/>
@@ -4739,10 +4828,10 @@
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
+      <c r="H80" s="54"/>
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
+      <c r="K80" s="7"/>
       <c r="L80" s="6"/>
       <c r="M80" s="6"/>
       <c r="N80" s="6"/>
@@ -4759,17 +4848,17 @@
     </row>
     <row r="81" spans="2:24" ht="15.75" customHeight="1">
       <c r="G81" s="6"/>
-      <c r="H81" s="64"/>
-      <c r="I81" s="65"/>
-      <c r="J81" s="65"/>
-      <c r="K81" s="65"/>
-      <c r="L81" s="65"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
       <c r="M81" s="6"/>
-      <c r="N81" s="127"/>
-      <c r="O81" s="126"/>
-      <c r="P81" s="126"/>
-      <c r="Q81" s="126"/>
-      <c r="R81" s="126"/>
+      <c r="N81" s="139"/>
+      <c r="O81" s="138"/>
+      <c r="P81" s="138"/>
+      <c r="Q81" s="138"/>
+      <c r="R81" s="138"/>
       <c r="S81" s="6"/>
       <c r="T81" s="6"/>
       <c r="U81" s="6"/>
@@ -4779,11 +4868,11 @@
     </row>
     <row r="82" spans="2:24" ht="15.75" customHeight="1">
       <c r="G82" s="6"/>
-      <c r="H82" s="64"/>
-      <c r="I82" s="65"/>
-      <c r="J82" s="65"/>
-      <c r="K82" s="65"/>
-      <c r="L82" s="65"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
       <c r="M82" s="6"/>
       <c r="N82" s="62"/>
       <c r="O82" s="62"/>
@@ -4799,11 +4888,11 @@
     </row>
     <row r="83" spans="2:24" ht="15.75" customHeight="1">
       <c r="G83" s="6"/>
-      <c r="H83" s="64"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
-      <c r="K83" s="65"/>
-      <c r="L83" s="65"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
       <c r="M83" s="6"/>
       <c r="N83" s="6"/>
       <c r="O83" s="6"/>
@@ -4838,6 +4927,11 @@
       <c r="X84" s="6"/>
     </row>
     <row r="85" spans="2:24" ht="15.75" customHeight="1">
+      <c r="H85" s="64"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="65"/>
+      <c r="L85" s="65"/>
       <c r="M85" s="6"/>
       <c r="S85" s="6"/>
       <c r="T85" s="6"/>
@@ -4847,6 +4941,11 @@
       <c r="X85" s="6"/>
     </row>
     <row r="86" spans="2:24" ht="15.75" customHeight="1">
+      <c r="H86" s="64"/>
+      <c r="I86" s="65"/>
+      <c r="J86" s="65"/>
+      <c r="K86" s="65"/>
+      <c r="L86" s="65"/>
       <c r="M86" s="6"/>
       <c r="S86" s="6"/>
       <c r="T86" s="6"/>
@@ -4856,6 +4955,11 @@
       <c r="X86" s="6"/>
     </row>
     <row r="87" spans="2:24" ht="15.75" customHeight="1">
+      <c r="H87" s="64"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="65"/>
+      <c r="K87" s="65"/>
+      <c r="L87" s="65"/>
       <c r="T87" s="6"/>
       <c r="U87" s="6"/>
       <c r="V87" s="6"/>
@@ -4888,11 +4992,11 @@
       <c r="F94" s="6"/>
     </row>
     <row r="95" spans="2:24" ht="15.75" customHeight="1">
-      <c r="B95" s="131"/>
-      <c r="C95" s="126"/>
-      <c r="D95" s="126"/>
-      <c r="E95" s="126"/>
-      <c r="F95" s="126"/>
+      <c r="B95" s="142"/>
+      <c r="C95" s="138"/>
+      <c r="D95" s="138"/>
+      <c r="E95" s="138"/>
+      <c r="F95" s="138"/>
     </row>
     <row r="96" spans="2:24" ht="15.75" customHeight="1">
       <c r="B96" s="73"/>
@@ -4903,41 +5007,31 @@
     </row>
     <row r="97" spans="7:24" ht="15.75" customHeight="1">
       <c r="G97" s="6"/>
-      <c r="H97" s="54"/>
-      <c r="I97" s="6"/>
-      <c r="J97" s="6"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="6"/>
     </row>
     <row r="98" spans="7:24" ht="15.75" customHeight="1">
       <c r="G98" s="6"/>
-      <c r="H98" s="54"/>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
-      <c r="K98" s="6"/>
-      <c r="L98" s="6"/>
     </row>
     <row r="99" spans="7:24" ht="15.75" customHeight="1">
       <c r="G99" s="6"/>
-      <c r="H99" s="54"/>
-      <c r="I99" s="6"/>
-      <c r="J99" s="6"/>
-      <c r="K99" s="6"/>
-      <c r="L99" s="6"/>
       <c r="M99" s="6"/>
       <c r="S99" s="6"/>
     </row>
     <row r="100" spans="7:24" ht="15.75" customHeight="1">
       <c r="G100" s="6"/>
-      <c r="H100" s="6"/>
+      <c r="H100" s="54"/>
       <c r="I100" s="6"/>
       <c r="J100" s="6"/>
-      <c r="K100" s="6"/>
+      <c r="K100" s="7"/>
       <c r="L100" s="6"/>
       <c r="M100" s="6"/>
       <c r="S100" s="6"/>
     </row>
     <row r="101" spans="7:24" ht="15.75" customHeight="1">
+      <c r="H101" s="54"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
       <c r="M101" s="6"/>
       <c r="S101" s="6"/>
       <c r="T101" s="71"/>
@@ -4947,10 +5041,20 @@
       <c r="X101" s="58"/>
     </row>
     <row r="102" spans="7:24" ht="15.75" customHeight="1">
+      <c r="H102" s="54"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
       <c r="M102" s="6"/>
       <c r="S102" s="6"/>
     </row>
     <row r="103" spans="7:24" ht="15.75" customHeight="1">
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
       <c r="M103" s="1"/>
       <c r="T103" s="6"/>
       <c r="U103" s="6"/>
@@ -5880,16 +5984,16 @@
     <row r="983" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="T65:X65"/>
+    <mergeCell ref="N81:R81"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B95:F95"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B48:F48"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="T65:X65"/>
-    <mergeCell ref="N81:R81"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="H21:L21"/>
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -5898,45 +6002,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" customWidth="1"/>
-    <col min="8" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="3.5703125" customWidth="1"/>
-    <col min="14" max="18" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="3.5546875" customWidth="1"/>
+    <col min="8" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" customWidth="1"/>
+    <col min="13" max="13" width="3.5546875" customWidth="1"/>
+    <col min="14" max="18" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="13.5" thickBot="1"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1">
+    <row r="1" spans="2:12" ht="13.8" thickBot="1"/>
+    <row r="2" spans="2:12" ht="14.4" thickBot="1">
       <c r="B2" s="143" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="142"/>
-      <c r="H2" s="128" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="133"/>
-    </row>
-    <row r="3" spans="2:12" ht="15">
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="136"/>
+      <c r="H2" s="125" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
+    </row>
+    <row r="3" spans="2:12" ht="13.8">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5968,7 +6072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="14.25">
+    <row r="4" spans="2:12" ht="14.4">
       <c r="B4" s="5" t="s">
         <v>107</v>
       </c>
@@ -5997,15 +6101,15 @@
         <v>20</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="14.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="14.4">
       <c r="B5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>10</v>
@@ -6014,13 +6118,13 @@
         <v>20</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>25</v>
@@ -6029,15 +6133,15 @@
         <v>10</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="14.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="14.4">
       <c r="B6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -6046,13 +6150,13 @@
         <v>60</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>25</v>
@@ -6064,12 +6168,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="14.25">
+    <row r="7" spans="2:12" ht="14.4">
       <c r="B7" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>10</v>
@@ -6078,13 +6182,13 @@
         <v>60</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>94</v>
@@ -6092,12 +6196,12 @@
       <c r="K7" s="7"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="2:12" ht="14.25">
+    <row r="8" spans="2:12" ht="14.4">
       <c r="B8" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>10</v>
@@ -6106,13 +6210,13 @@
         <v>30</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>94</v>
@@ -6120,25 +6224,25 @@
       <c r="K8" s="7"/>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="2:12" ht="14.25">
+    <row r="9" spans="2:12" ht="14.4">
       <c r="B9" s="44" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D9" s="45" t="s">
         <v>94</v>
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="53" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>25</v>
@@ -6152,13 +6256,13 @@
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1">
       <c r="B10" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E10" s="18">
         <v>1</v>
@@ -6167,10 +6271,10 @@
         <v>28</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>10</v>
@@ -6179,12 +6283,12 @@
         <v>10</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="14.4" thickBot="1">
       <c r="B11" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>58</v>
@@ -6197,12 +6301,12 @@
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="2:12" ht="15">
+    <row r="12" spans="2:12" ht="13.8">
       <c r="B12" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>10</v>
@@ -6211,19 +6315,19 @@
         <v>15</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H12" s="143" t="s">
-        <v>158</v>
-      </c>
-      <c r="I12" s="141"/>
-      <c r="J12" s="141"/>
-      <c r="K12" s="141"/>
-      <c r="L12" s="142"/>
-    </row>
-    <row r="13" spans="2:12" ht="15">
+        <v>155</v>
+      </c>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="136"/>
+    </row>
+    <row r="13" spans="2:12" ht="13.8">
       <c r="B13" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
@@ -6251,12 +6355,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="14.25">
+    <row r="14" spans="2:12" ht="14.4">
       <c r="B14" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>10</v>
@@ -6266,10 +6370,10 @@
       </c>
       <c r="F14" s="8"/>
       <c r="H14" s="50" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J14" s="37" t="s">
         <v>10</v>
@@ -6281,12 +6385,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="14.25">
+    <row r="15" spans="2:12" ht="14.4">
       <c r="B15" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>10</v>
@@ -6295,10 +6399,10 @@
         <v>50</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>108</v>
@@ -6313,15 +6417,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="14.25">
+    <row r="16" spans="2:12" ht="14.4">
       <c r="B16" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E16" s="18">
         <v>1</v>
@@ -6330,7 +6434,7 @@
         <v>28</v>
       </c>
       <c r="H16" s="51" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>9</v>
@@ -6345,15 +6449,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="14.25">
+    <row r="17" spans="2:12" ht="14.4">
       <c r="B17" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E17" s="18">
         <v>1</v>
@@ -6362,10 +6466,10 @@
         <v>28</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>25</v>
@@ -6375,12 +6479,12 @@
       </c>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:12" ht="14.25">
+    <row r="18" spans="2:12" ht="14.4">
       <c r="B18" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>94</v>
@@ -6388,10 +6492,10 @@
       <c r="E18" s="47"/>
       <c r="F18" s="8"/>
       <c r="H18" s="50" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>10</v>
@@ -6401,12 +6505,12 @@
       </c>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:12" ht="17.25" thickBot="1">
+    <row r="19" spans="2:12" ht="18" thickBot="1">
       <c r="B19" s="14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>94</v>
@@ -6414,10 +6518,10 @@
       <c r="E19" s="48"/>
       <c r="F19" s="13"/>
       <c r="H19" s="50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>25</v>
@@ -6427,12 +6531,12 @@
       </c>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:12" ht="14.25">
+    <row r="20" spans="2:12" ht="14.4">
       <c r="H20" s="50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>94</v>
@@ -6442,10 +6546,10 @@
     </row>
     <row r="21" spans="2:12" ht="15" thickBot="1">
       <c r="H21" s="55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>94</v>
@@ -6453,17 +6557,17 @@
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="2:12" ht="13.5" thickBot="1"/>
-    <row r="23" spans="2:12" ht="15">
-      <c r="H23" s="137" t="s">
-        <v>159</v>
-      </c>
-      <c r="I23" s="135"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="135"/>
-      <c r="L23" s="136"/>
-    </row>
-    <row r="24" spans="2:12" ht="15">
+    <row r="22" spans="2:12" ht="13.8" thickBot="1"/>
+    <row r="23" spans="2:12" ht="13.8">
+      <c r="H23" s="131" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
+      <c r="K23" s="129"/>
+      <c r="L23" s="130"/>
+    </row>
+    <row r="24" spans="2:12" ht="13.8">
       <c r="H24" s="96" t="s">
         <v>3</v>
       </c>
@@ -6480,12 +6584,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="14.25">
+    <row r="25" spans="2:12" ht="14.4">
       <c r="H25" s="98" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I25" s="94" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J25" s="94" t="s">
         <v>25</v>
@@ -6494,15 +6598,15 @@
         <v>15</v>
       </c>
       <c r="L25" s="99" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="14.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="14.4">
       <c r="H26" s="98" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I26" s="94" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J26" s="94" t="s">
         <v>25</v>
@@ -6511,10 +6615,10 @@
         <v>15</v>
       </c>
       <c r="L26" s="99" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" ht="14.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="14.4">
       <c r="H27" s="98" t="s">
         <v>109</v>
       </c>
@@ -6526,15 +6630,15 @@
       </c>
       <c r="K27" s="95"/>
       <c r="L27" s="100" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="14.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="14.4">
       <c r="H28" s="98" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I28" s="94" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J28" s="94" t="s">
         <v>25</v>
@@ -6546,12 +6650,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="14.25">
+    <row r="29" spans="2:12" ht="14.4">
       <c r="H29" s="98" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I29" s="94" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J29" s="94" t="s">
         <v>25</v>
@@ -6560,15 +6664,15 @@
         <v>10</v>
       </c>
       <c r="L29" s="100" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" ht="14.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="14.4">
       <c r="H30" s="98" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I30" s="94" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J30" s="94" t="s">
         <v>94</v>
@@ -6576,12 +6680,12 @@
       <c r="K30" s="95"/>
       <c r="L30" s="100"/>
     </row>
-    <row r="31" spans="2:12" ht="14.25">
+    <row r="31" spans="2:12" ht="14.4">
       <c r="H31" s="98" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I31" s="94" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J31" s="94" t="s">
         <v>25</v>
@@ -6590,15 +6694,15 @@
         <v>10</v>
       </c>
       <c r="L31" s="100" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="14.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="14.4">
       <c r="H32" s="98" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I32" s="94" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J32" s="94" t="s">
         <v>25</v>
@@ -6607,32 +6711,32 @@
         <v>10</v>
       </c>
       <c r="L32" s="100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="8:12" ht="14.4">
+      <c r="H33" s="98" t="s">
+        <v>203</v>
+      </c>
+      <c r="I33" s="94" t="s">
+        <v>204</v>
+      </c>
+      <c r="J33" s="94" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="33" spans="8:12" ht="14.25">
-      <c r="H33" s="98" t="s">
+      <c r="K33" s="95">
+        <v>10</v>
+      </c>
+      <c r="L33" s="100" t="s">
         <v>206</v>
       </c>
-      <c r="I33" s="94" t="s">
+    </row>
+    <row r="34" spans="8:12" ht="14.4">
+      <c r="H34" s="98" t="s">
         <v>207</v>
       </c>
-      <c r="J33" s="94" t="s">
+      <c r="I34" s="94" t="s">
         <v>208</v>
-      </c>
-      <c r="K33" s="95">
-        <v>10</v>
-      </c>
-      <c r="L33" s="100" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="8:12" ht="14.25">
-      <c r="H34" s="98" t="s">
-        <v>210</v>
-      </c>
-      <c r="I34" s="94" t="s">
-        <v>211</v>
       </c>
       <c r="J34" s="94" t="s">
         <v>10</v>
@@ -6644,10 +6748,10 @@
     </row>
     <row r="35" spans="8:12" ht="15" thickBot="1">
       <c r="H35" s="101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I35" s="102" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J35" s="102" t="s">
         <v>10</v>
@@ -6671,55 +6775,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.88671875" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="13.5" thickBot="1"/>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B2" s="128" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="133"/>
+    <row r="1" spans="2:18" ht="13.8" thickBot="1"/>
+    <row r="2" spans="2:18" ht="14.4" thickBot="1">
+      <c r="B2" s="125" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="127"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="128" t="s">
-        <v>216</v>
-      </c>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="133"/>
+      <c r="H2" s="125" t="s">
+        <v>213</v>
+      </c>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="128" t="s">
-        <v>251</v>
-      </c>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="133"/>
-    </row>
-    <row r="3" spans="2:18" ht="15">
+      <c r="N2" s="125" t="s">
+        <v>248</v>
+      </c>
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="126"/>
+      <c r="R2" s="127"/>
+    </row>
+    <row r="3" spans="2:18" ht="13.8">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -6768,12 +6872,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="15">
+    <row r="4" spans="2:18" ht="13.8">
       <c r="B4" s="30" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>25</v>
@@ -6786,10 +6890,10 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="30" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>25</v>
@@ -6802,10 +6906,10 @@
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="30" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>25</v>
@@ -6817,12 +6921,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="15">
+    <row r="5" spans="2:18" ht="13.8">
       <c r="B5" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>10</v>
@@ -6835,10 +6939,10 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>10</v>
@@ -6847,14 +6951,14 @@
         <v>60</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>10</v>
@@ -6866,12 +6970,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="14.25">
+    <row r="6" spans="2:18" ht="13.8">
       <c r="B6" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -6884,10 +6988,10 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>10</v>
@@ -6900,10 +7004,10 @@
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>10</v>
@@ -6915,12 +7019,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="14.25">
+    <row r="7" spans="2:18" ht="13.8">
       <c r="B7" s="30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>94</v>
@@ -6929,10 +7033,10 @@
       <c r="F7" s="8"/>
       <c r="G7" s="6"/>
       <c r="H7" s="30" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>10</v>
@@ -6941,14 +7045,14 @@
         <v>15</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>94</v>
@@ -6956,12 +7060,12 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="2:18" ht="14.25">
+    <row r="8" spans="2:18" ht="13.8">
       <c r="B8" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>10</v>
@@ -6974,13 +7078,13 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="8"/>
@@ -7001,25 +7105,25 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="14.25">
+    <row r="9" spans="2:18" ht="13.8">
       <c r="B9" s="30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="30" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>108</v>
@@ -7035,10 +7139,10 @@
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>94</v>
@@ -7046,12 +7150,12 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1">
+    <row r="10" spans="2:18" ht="14.4" thickBot="1">
       <c r="B10" s="70" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>10</v>
@@ -7062,26 +7166,26 @@
       <c r="F10" s="13"/>
       <c r="G10" s="6"/>
       <c r="H10" s="30" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K10" s="7">
         <v>1</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="30" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>25</v>
@@ -7090,10 +7194,10 @@
         <v>2</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" ht="15" thickBot="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="14.4" thickBot="1">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -7101,10 +7205,10 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="30" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>10</v>
@@ -7115,7 +7219,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="6"/>
       <c r="N11" s="30" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O11" s="6" t="s">
         <v>108</v>
@@ -7130,20 +7234,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B12" s="128" t="s">
-        <v>215</v>
-      </c>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="133"/>
+    <row r="12" spans="2:18" ht="14.4" thickBot="1">
+      <c r="B12" s="125" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="127"/>
       <c r="G12" s="6"/>
       <c r="H12" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>94</v>
@@ -7152,10 +7256,10 @@
       <c r="L12" s="8"/>
       <c r="M12" s="6"/>
       <c r="N12" s="70" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="O12" s="75" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="P12" s="75" t="s">
         <v>10</v>
@@ -7165,7 +7269,7 @@
       </c>
       <c r="R12" s="69"/>
     </row>
-    <row r="13" spans="2:18" ht="15.75" thickBot="1">
+    <row r="13" spans="2:18" ht="14.4" thickBot="1">
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
@@ -7183,10 +7287,10 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="70" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>10</v>
@@ -7197,12 +7301,12 @@
       <c r="L13" s="13"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="2:18" ht="15" thickBot="1">
+    <row r="14" spans="2:18" ht="14.4" thickBot="1">
       <c r="B14" s="30" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>25</v>
@@ -7214,12 +7318,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1">
+    <row r="15" spans="2:18" ht="15" thickBot="1">
       <c r="B15" s="66" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>10</v>
@@ -7231,20 +7335,20 @@
         <v>24</v>
       </c>
       <c r="H15" s="146" t="s">
-        <v>284</v>
-      </c>
-      <c r="I15" s="132"/>
-      <c r="J15" s="132"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="133"/>
+        <v>281</v>
+      </c>
+      <c r="I15" s="126"/>
+      <c r="J15" s="126"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="127"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="2:18" ht="15">
+    <row r="16" spans="2:18" ht="13.8">
       <c r="B16" s="66" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>10</v>
@@ -7272,12 +7376,12 @@
       </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" ht="14.25">
+    <row r="17" spans="2:13" ht="14.4">
       <c r="B17" s="30" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>10</v>
@@ -7289,10 +7393,10 @@
         <v>24</v>
       </c>
       <c r="H17" s="80" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I17" s="81" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>25</v>
@@ -7301,16 +7405,16 @@
         <v>3</v>
       </c>
       <c r="L17" s="82" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="2:13" ht="14.25">
+    <row r="18" spans="2:13" ht="13.8">
       <c r="B18" s="66" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>10</v>
@@ -7319,36 +7423,36 @@
         <v>30</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H18" s="80" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I18" s="81" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J18" s="81" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K18" s="19">
         <v>10</v>
       </c>
       <c r="L18" s="82" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="2:13" ht="15" thickBot="1">
+    <row r="19" spans="2:13" ht="14.4" thickBot="1">
       <c r="B19" s="67"/>
       <c r="C19" s="68"/>
       <c r="D19" s="68"/>
       <c r="E19" s="68"/>
       <c r="F19" s="69"/>
       <c r="H19" s="30" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>10</v>
@@ -7361,12 +7465,12 @@
       </c>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="2:13" ht="15" thickBot="1">
+    <row r="20" spans="2:13" ht="14.4" thickBot="1">
       <c r="H20" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>10</v>
@@ -7379,19 +7483,19 @@
       </c>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="2:13" ht="15.75" thickBot="1">
+    <row r="21" spans="2:13" ht="15" thickBot="1">
       <c r="B21" s="145" t="s">
-        <v>283</v>
-      </c>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="133"/>
+        <v>280</v>
+      </c>
+      <c r="C21" s="126"/>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="127"/>
       <c r="H21" s="30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>94</v>
@@ -7400,7 +7504,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="2:13" ht="15">
+    <row r="22" spans="2:13" ht="13.8">
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
@@ -7417,7 +7521,7 @@
         <v>7</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>108</v>
@@ -7435,10 +7539,10 @@
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1">
       <c r="B23" s="80" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>25</v>
@@ -7447,13 +7551,13 @@
         <v>3</v>
       </c>
       <c r="F23" s="82" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H23" s="70" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>10</v>
@@ -7464,12 +7568,12 @@
       <c r="L23" s="13"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="2:13" ht="15" thickBot="1">
+    <row r="24" spans="2:13" ht="14.4" thickBot="1">
       <c r="B24" s="77" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>10</v>
@@ -7481,12 +7585,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="15.75" thickBot="1">
+    <row r="25" spans="2:13" ht="15.6" thickBot="1">
       <c r="B25" s="78" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C25" s="79" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>10</v>
@@ -7498,14 +7602,14 @@
         <v>24</v>
       </c>
       <c r="H25" s="146" t="s">
-        <v>285</v>
-      </c>
-      <c r="I25" s="132"/>
-      <c r="J25" s="132"/>
-      <c r="K25" s="132"/>
-      <c r="L25" s="133"/>
-    </row>
-    <row r="26" spans="2:13" ht="15.75" thickBot="1">
+        <v>282</v>
+      </c>
+      <c r="I25" s="126"/>
+      <c r="J25" s="126"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="127"/>
+    </row>
+    <row r="26" spans="2:13" ht="14.4" thickBot="1">
       <c r="B26" s="54"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -7527,31 +7631,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="15.75" thickBot="1">
+    <row r="27" spans="2:13" ht="16.2" thickBot="1">
       <c r="B27" s="144" t="s">
-        <v>282</v>
-      </c>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="133"/>
+        <v>279</v>
+      </c>
+      <c r="C27" s="126"/>
+      <c r="D27" s="126"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="127"/>
       <c r="H27" s="85" t="s">
+        <v>270</v>
+      </c>
+      <c r="I27" s="83" t="s">
         <v>273</v>
       </c>
-      <c r="I27" s="83" t="s">
-        <v>276</v>
-      </c>
       <c r="J27" s="83" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K27" s="74">
         <v>10</v>
       </c>
       <c r="L27" s="84" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" ht="15">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="13.8">
       <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
@@ -7568,10 +7672,10 @@
         <v>7</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>25</v>
@@ -7583,12 +7687,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="14.25">
+    <row r="29" spans="2:13" ht="13.8">
       <c r="B29" s="80" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>25</v>
@@ -7597,13 +7701,13 @@
         <v>3</v>
       </c>
       <c r="F29" s="82" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>10</v>
@@ -7612,15 +7716,15 @@
         <v>500</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" ht="15" thickBot="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="14.4" thickBot="1">
       <c r="B30" s="90" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C30" s="87" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D30" s="88" t="s">
         <v>10</v>
@@ -7632,7 +7736,7 @@
         <v>24</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>108</v>
@@ -7644,18 +7748,18 @@
         <v>20</v>
       </c>
       <c r="L30" s="82" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" ht="15" thickBot="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="14.4" thickBot="1">
       <c r="H31" s="70" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="13"/>
@@ -7677,32 +7781,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="13.5" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B2" s="128" t="s">
+    <row r="1" spans="2:6" ht="13.8" thickBot="1"/>
+    <row r="2" spans="2:6" ht="15" thickBot="1">
+      <c r="B2" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="133"/>
-    </row>
-    <row r="3" spans="2:6" ht="15">
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="127"/>
+    </row>
+    <row r="3" spans="2:6" ht="13.8">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -7719,7 +7823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="14.25">
+    <row r="4" spans="2:6" ht="14.4">
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
@@ -7736,7 +7840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="14.25">
+    <row r="5" spans="2:6" ht="14.4">
       <c r="B5" s="5" t="s">
         <v>22</v>
       </c>

</xml_diff>